<commit_message>
updated file in budget folder
</commit_message>
<xml_diff>
--- a/budget/budget.xlsx
+++ b/budget/budget.xlsx
@@ -1,28 +1,131 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b92c255fc56e8351/Documents/CITE/Projects/pm-s04-g04-project/budget/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="168" documentId="11_F25DC773A252ABDACC104828B95C64BE5BDE58F6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E4064279-E970-4790-98C3-C5A5B276F485}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t>Budget for Resources</t>
+  </si>
+  <si>
+    <t>Number of Units</t>
+  </si>
+  <si>
+    <t>Systems</t>
+  </si>
+  <si>
+    <t>Servers</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Cost per Unit</t>
+  </si>
+  <si>
+    <t>Budget for Equipment</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Hourly Pay</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total for Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Project Manager</t>
+  </si>
+  <si>
+    <t>Systems  Administrator</t>
+  </si>
+  <si>
+    <t>Software Administator</t>
+  </si>
+  <si>
+    <t>Project Coordinator</t>
+  </si>
+  <si>
+    <t>Hours per Week</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Total for Resources</t>
+  </si>
+  <si>
+    <t>Total Budget for Project</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -46,13 +149,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +457,433 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>150</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7">
+        <v>499</v>
+      </c>
+      <c r="F3" s="7">
+        <f>B3*E3</f>
+        <v>74850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7">
+        <v>1200</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" ref="F4:F5" si="0">B4*E4</f>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7">
+        <v>99</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8">
+        <f>SUM(F3:F5)</f>
+        <v>115800</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="10" spans="1:20" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <f>8*5</f>
+        <v>40</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7">
+        <v>80</v>
+      </c>
+      <c r="F12" s="7">
+        <f>B12*E12</f>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4">
+        <f>15*5</f>
+        <v>75</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7">
+        <v>75</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" ref="F13:F15" si="1">B13*E13</f>
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <f>30*5</f>
+        <v>150</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7">
+        <v>40</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <f>30*5</f>
+        <v>150</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7">
+        <v>45</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="1"/>
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8">
+        <f>SUM(F12:F15)</f>
+        <v>21575</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8">
+        <f>SUM(B7,B17)</f>
+        <v>137375</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006F8EAAD027AD2438921658AEAA4D94D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="913b181d90f3e37837a166d2920f8a4b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b96ae70f-2898-427b-8338-a4af5c833311" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2960af4209ceb4cd24dc8db11711d6ad" ns2:_="">
+    <xsd:import namespace="b96ae70f-2898-427b-8338-a4af5c833311"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b96ae70f-2898-427b-8338-a4af5c833311" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73839E34-7FDB-44BE-81C9-CED8BB93C16A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53494AB6-9932-4DB1-B6B2-9341235F4E86}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41E72BA-B270-48C4-9024-4A64A84B7B67}"/>
 </file>
</xml_diff>

<commit_message>
added budgert file to folder
</commit_message>
<xml_diff>
--- a/budget/budget.xlsx
+++ b/budget/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b92c255fc56e8351/Documents/CITE/Projects/pm-s04-g04-project/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="11_F25DC773A252ABDACC104828B95C64BE5BDE58F6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E4064279-E970-4790-98C3-C5A5B276F485}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="11_F25DC773A252ABDACC104828B95C64BE5BDE58F6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{94A2D494-D927-4D1B-93F5-8DEA2AE5C639}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,26 +155,26 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -461,53 +461,53 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -515,15 +515,15 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="9">
         <v>150</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="5">
         <v>499</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <f>B3*E3</f>
         <v>74850</v>
       </c>
@@ -532,15 +532,15 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="9">
         <v>30</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="5">
         <v>1200</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <f t="shared" ref="F4:F5" si="0">B4*E4</f>
         <v>36000</v>
       </c>
@@ -549,62 +549,62 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="9">
         <v>50</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="5">
         <v>99</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>4950</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="10">
         <f>SUM(F3:F5)</f>
         <v>115800</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="10" spans="1:20" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="10" spans="1:20" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -612,117 +612,113 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
-        <f>8*5</f>
-        <v>40</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7">
-        <v>80</v>
-      </c>
-      <c r="F12" s="7">
-        <f>B12*E12</f>
-        <v>3200</v>
+      <c r="B12" s="9">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="5">
+        <v>70</v>
+      </c>
+      <c r="F12" s="5">
+        <f>E12*B12*10</f>
+        <v>3500</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4">
-        <f>15*5</f>
-        <v>75</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7">
-        <v>75</v>
-      </c>
-      <c r="F13" s="7">
-        <f t="shared" ref="F13:F15" si="1">B13*E13</f>
-        <v>5625</v>
+      <c r="B13" s="9">
+        <v>8</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="5">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" ref="F13:F15" si="1">E13*B13*10</f>
+        <v>4400</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
-        <f>30*5</f>
-        <v>150</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7">
-        <v>40</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="B14" s="9">
+        <v>20</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="5">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
-        <f>30*5</f>
-        <v>150</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7">
-        <v>45</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="B15" s="9">
+        <v>20</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="5">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
-        <v>6750</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="10">
         <f>SUM(F12:F15)</f>
-        <v>21575</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+        <v>27900</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="10">
         <f>SUM(B7,B17)</f>
-        <v>137375</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+        <v>143700</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -730,8 +726,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006F8EAAD027AD2438921658AEAA4D94D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="913b181d90f3e37837a166d2920f8a4b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b96ae70f-2898-427b-8338-a4af5c833311" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2960af4209ceb4cd24dc8db11711d6ad" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006F8EAAD027AD2438921658AEAA4D94D" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="384915d2e0e91aae6811ba7382d4329e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b96ae70f-2898-427b-8338-a4af5c833311" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc046178f20e8478d62e020d184eaee9" ns2:_="">
     <xsd:import namespace="b96ae70f-2898-427b-8338-a4af5c833311"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -741,6 +737,10 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -759,6 +759,28 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -877,13 +899,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73839E34-7FDB-44BE-81C9-CED8BB93C16A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27A5C78B-7E6B-4EE0-9694-8D3817CA39BC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53494AB6-9932-4DB1-B6B2-9341235F4E86}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53494AB6-9932-4DB1-B6B2-9341235F4E86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41E72BA-B270-48C4-9024-4A64A84B7B67}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41E72BA-B270-48C4-9024-4A64A84B7B67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>